<commit_message>
Implementation for only_score agents
</commit_message>
<xml_diff>
--- a/models/models.xlsx
+++ b/models/models.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -110,24 +110,15 @@
     <t>Seems to imitate the baseline agent well, but gets confused when attacking. This is probably, because the agent can't differenciate properly if it is attacking or defening</t>
   </si>
   <si>
-    <t>-1 if action is STOP. Changes the reward depending on if the agent recovered food from the rival, or if it returned food.</t>
-  </si>
-  <si>
     <t>Learns to defend, but not to attack</t>
   </si>
   <si>
-    <t>random_actions_differenciates_pacman</t>
-  </si>
-  <si>
     <t>-0.5 is action is STOP. Changes the reward depending on if the agent recovered food from the rival. 2*number of returned food. -food lost if the agent was eaten. Score changes</t>
   </si>
   <si>
     <t>Took 65149.9921788</t>
   </si>
   <si>
-    <t>baseline_actions_differenciates_pacman2</t>
-  </si>
-  <si>
     <t>Took 49159.3473346</t>
   </si>
   <si>
@@ -135,6 +126,51 @@
   </si>
   <si>
     <t>Learns to defend on both sides. Doesn't attack</t>
+  </si>
+  <si>
+    <t>random_actions_distinguishes_pacman</t>
+  </si>
+  <si>
+    <t>baseline_actions_distinguishes_pacman2</t>
+  </si>
+  <si>
+    <t>random_actions_only_score</t>
+  </si>
+  <si>
+    <t>baseline_actions_only_score</t>
+  </si>
+  <si>
+    <t>Score change. +n for n returned food</t>
+  </si>
+  <si>
+    <t>Took 56900.1227956</t>
+  </si>
+  <si>
+    <t>Took 63154.4934079</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>A baseline</t>
+  </si>
+  <si>
+    <t>A random</t>
+  </si>
+  <si>
+    <t>B random</t>
+  </si>
+  <si>
+    <t>B baseline</t>
+  </si>
+  <si>
+    <t>C random</t>
+  </si>
+  <si>
+    <t>C baseline</t>
+  </si>
+  <si>
+    <t>-0.5 if action is STOP. Changes the reward depending on if the agent recovered food from the rival, or if it returned food.</t>
   </si>
 </sst>
 </file>
@@ -189,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -214,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,242 +531,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" customWidth="1"/>
-    <col min="5" max="5" width="62.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="62.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>1500000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>1500000</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>1500000</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1500000</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="G8" s="11">
         <v>1500000</v>
       </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10">
         <v>1500000</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="H10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="13" t="s">
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11">
+        <v>1500000</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13">
         <v>1500000</v>
       </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11">
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14">
         <v>1500000</v>
       </c>
-      <c r="G11" t="s">
-        <v>34</v>
+      <c r="H14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>